<commit_message>
Minor wire harness updates
</commit_message>
<xml_diff>
--- a/Antonio-Feed/Wiring Harnesses/Feed/Dewar Communication Cable (Triple Cable)/List of materials (triple cable).xlsx
+++ b/Antonio-Feed/Wiring Harnesses/Feed/Dewar Communication Cable (Triple Cable)/List of materials (triple cable).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah/Documents/GitHub/Front-Page/Antonio-Feed/Wiring Harnesses/Feed/Dewar Communication Cable (Triple Cable)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02700308-BD68-D645-957E-109BB5906336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EACEE3D-0274-EA4D-9827-4B6BC6888D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12900" yWindow="1800" windowWidth="22940" windowHeight="12280" xr2:uid="{1354B1EE-61B1-EA40-838A-2C3EED4877E0}"/>
   </bookViews>
@@ -887,8 +887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BA75E2-A133-C247-9618-E9CB2A5F5006}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26:G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1245,7 +1245,7 @@
         <v>111</v>
       </c>
       <c r="C13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>88</v>
@@ -1274,7 +1274,7 @@
         <v>111</v>
       </c>
       <c r="C14" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>88</v>

</xml_diff>